<commit_message>
Few More Problems Solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\Babbars-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CCCE57-6D00-4B30-ADD0-37372CFB5D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E8A569-9E3C-447D-8CD7-4FDA2B378E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
Few more matrix questions solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\Babbars-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E8A569-9E3C-447D-8CD7-4FDA2B378E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1530AF44-C399-43F9-B89B-A67548D6F214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1428,6 +1428,12 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>Largest Rectangular Area in a Histogram</t>
+  </si>
+  <si>
+    <t>Zigzag (or diagonal) traversal of Matrix</t>
   </si>
 </sst>
 </file>
@@ -1518,7 +1524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1542,6 +1548,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1859,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1927,7 +1939,7 @@
     </row>
     <row r="8" spans="1:4" ht="21">
       <c r="A8">
-        <f t="shared" ref="A8:A41" si="0">A7+1</f>
+        <f t="shared" ref="A8:A42" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2436,7 +2448,16 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="21">
-      <c r="C42" s="7"/>
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>465</v>
+      </c>
       <c r="D42" s="4" t="s">
         <v>4</v>
       </c>
@@ -2479,7 +2500,7 @@
     </row>
     <row r="46" spans="1:4" ht="21">
       <c r="A46">
-        <f t="shared" ref="A46:A53" si="1">A45+1</f>
+        <f t="shared" ref="A46:A54" si="1">A45+1</f>
         <v>3</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -2595,6 +2616,18 @@
       </c>
       <c r="D53" s="4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="21">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -8611,7 +8644,10 @@
     <hyperlink ref="C480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="C356" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="C2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
+    <hyperlink ref="C42" r:id="rId447" xr:uid="{E3C7C778-400E-4040-8C40-EB13BAE7335A}"/>
+    <hyperlink ref="C54" r:id="rId448" xr:uid="{D63F5A5F-094C-45DC-8BA6-D7BE5581DA1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId449"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Few String Problems Solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\Babbars-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFC03D3-FA55-451F-93E3-98326BBA82BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3D37F3-5B0E-459A-8B20-14FD37ABADEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1537,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1575,6 +1575,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1892,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2835,18 +2839,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="21">
-      <c r="A68">
+    <row r="68" spans="1:4" s="13" customFormat="1" ht="21">
+      <c r="A68" s="13">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="16" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Few LinkList Problems Solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\Babbars-Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\DSA-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDF0D0F-A997-41DB-BE24-B2B5329E7837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F621183-07BA-4489-90D6-DB38FBFA5B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1896,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
Binary Tree Problems Solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\DSA-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F621183-07BA-4489-90D6-DB38FBFA5B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4236F18A-0651-441F-BD64-6DD36464F276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1510,7 +1510,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1520,6 +1520,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1537,7 +1543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1575,10 +1581,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1896,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2839,18 +2849,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="13" customFormat="1" ht="21">
-      <c r="A68" s="13">
+    <row r="68" spans="1:4" s="17" customFormat="1" ht="21">
+      <c r="A68" s="17">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="20" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Few BST problems solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\DSA-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4236F18A-0651-441F-BD64-6DD36464F276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E912FC1-BA4C-4F97-BA90-1D81EA2FCAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1434,6 +1434,9 @@
   </si>
   <si>
     <t>Rotate matrix by 90 degrees (Clockwise and anticlockwise)</t>
+  </si>
+  <si>
+    <t>Sorted Array to BST</t>
   </si>
 </sst>
 </file>
@@ -1906,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="C232" sqref="C232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5269,7 +5272,15 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="21">
-      <c r="C236" s="7"/>
+      <c r="A236">
+        <v>23</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C236" s="6" t="s">
+        <v>467</v>
+      </c>
       <c r="D236" s="4"/>
     </row>
     <row r="237" spans="1:4" ht="21">
@@ -8681,8 +8692,9 @@
     <hyperlink ref="C2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="C42" r:id="rId447" xr:uid="{E3C7C778-400E-4040-8C40-EB13BAE7335A}"/>
     <hyperlink ref="C54" r:id="rId448" xr:uid="{D63F5A5F-094C-45DC-8BA6-D7BE5581DA1D}"/>
+    <hyperlink ref="C236" r:id="rId449" xr:uid="{27C9C804-31C5-4DD6-838B-B1DB78F95E7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId449"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId450"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search Tree Problems Solved
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Engineering\SE COMP 2020\Data Structures\DSA-Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E912FC1-BA4C-4F97-BA90-1D81EA2FCAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33635CEF-2FED-4BC5-ADA9-85DBF07740D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1546,7 +1546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1592,6 +1592,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1909,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="C232" sqref="C232"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="C211" sqref="C211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4632,18 +4636,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="21">
-      <c r="A192">
+    <row r="192" spans="1:4" s="13" customFormat="1" ht="21">
+      <c r="A192" s="13">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="B192" s="5" t="s">
+      <c r="B192" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="C192" s="6" t="s">
+      <c r="C192" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="D192" s="4" t="s">
+      <c r="D192" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5181,33 +5185,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="21">
-      <c r="A230">
+    <row r="230" spans="1:4" s="13" customFormat="1" ht="21">
+      <c r="A230" s="13">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="B230" s="5" t="s">
+      <c r="B230" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C230" s="6" t="s">
+      <c r="C230" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="D230" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" ht="21">
-      <c r="A231">
+      <c r="D230" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" s="13" customFormat="1" ht="21">
+      <c r="A231" s="13">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="B231" s="5" t="s">
+      <c r="B231" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C231" s="6" t="s">
+      <c r="C231" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="D231" s="4" t="s">
+      <c r="D231" s="16" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>